<commit_message>
New calibration of hx711. Added datasheets and other docs.
</commit_message>
<xml_diff>
--- a/breadbot/MeasureGainForScale.xlsx
+++ b/breadbot/MeasureGainForScale.xlsx
@@ -16,15 +16,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>scale</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>referenz</t>
   </si>
   <si>
     <t>get_unit</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>S-</t>
+  </si>
+  <si>
+    <t>E-</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>S+</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>E+</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>Test der Widerstände in der LoadCell</t>
+  </si>
+  <si>
+    <t>Fazit</t>
+  </si>
+  <si>
+    <t>sind ausgeglichen, sollte passen</t>
+  </si>
+  <si>
+    <t>Quelle</t>
+  </si>
+  <si>
+    <t>https://forum.arduino.cc/index.php?topic=320271.0</t>
+  </si>
+  <si>
+    <t>SCALE</t>
+  </si>
+  <si>
+    <t>Anstieg</t>
+  </si>
+  <si>
+    <t>OFFSET</t>
+  </si>
+  <si>
+    <t>SCALE*</t>
+  </si>
+  <si>
+    <t>Kalibrierung mit 3 Bierflaschen (immer in gleicher reihenfolge draufstellen, die flaschen haben ca. 5 g abweichung)</t>
+  </si>
+  <si>
+    <t>Iteratives Vorgehen</t>
+  </si>
+  <si>
+    <t>Start mit CalibrationFactor (SCALE) = 1</t>
+  </si>
+  <si>
+    <t>Fazit:</t>
+  </si>
+  <si>
+    <t>durchgängig 2 g abweichung nach letzter Messung -&gt; passt</t>
   </si>
 </sst>
 </file>
@@ -40,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -60,8 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -116,36 +190,36 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$4</c:f>
+              <c:f>Tabelle1!$A$16:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>362</c:v>
+                  <c:v>366540</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>725</c:v>
+                  <c:v>728367</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1086</c:v>
+                  <c:v>1089191</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$4</c:f>
+              <c:f>Tabelle1!$B$16:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>884</c:v>
+                  <c:v>892</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1779</c:v>
+                  <c:v>1778</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2664</c:v>
+                  <c:v>2678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -160,11 +234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93603520"/>
-        <c:axId val="93602944"/>
+        <c:axId val="51684480"/>
+        <c:axId val="51685056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93603520"/>
+        <c:axId val="51684480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -174,12 +248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93602944"/>
+        <c:crossAx val="51685056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93602944"/>
+        <c:axId val="51685056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -190,7 +264,291 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93603520"/>
+        <c:crossAx val="51684480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$25:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>913</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$25:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="51686784"/>
+        <c:axId val="51687936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="51686784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51687936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="51687936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51686784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$36:$A$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1776</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$36:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="99288192"/>
+        <c:axId val="100386496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="99288192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100386496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="100386496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99288192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -216,21 +574,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -246,22 +606,22 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2714625" cy="264560"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="Textfeld 5"/>
+            <xdr:cNvPr id="7" name="Textfeld 6"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3219449" y="938212"/>
+              <a:off x="2724149" y="2243137"/>
               <a:ext cx="2714625" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -289,6 +649,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -336,12 +697,12 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="Textfeld 5"/>
+            <xdr:cNvPr id="7" name="Textfeld 6"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3219449" y="938212"/>
+              <a:off x="2724149" y="2243137"/>
               <a:ext cx="2714625" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -369,6 +730,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="de-DE" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
@@ -383,6 +745,70 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagramm 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagramm 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -673,53 +1099,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D6"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>43476</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E4">
+        <v>269</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>270</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>270</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>362</v>
-      </c>
-      <c r="D2">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>725</v>
-      </c>
-      <c r="D3">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1086</v>
-      </c>
-      <c r="D4">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="D6">
-        <f>1000/2.4525</f>
-        <v>407.74719673802241</v>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>366540</v>
+      </c>
+      <c r="B16">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>728367</v>
+      </c>
+      <c r="B17">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1089191</v>
+      </c>
+      <c r="B18">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f>1/B20</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>322342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-0.3</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>913</v>
+      </c>
+      <c r="B26">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1816</v>
+      </c>
+      <c r="B27">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2716</v>
+      </c>
+      <c r="B28">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <v>0.98340000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <f>1/B30</f>
+        <v>1.016880211511084</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <f>B21*B31</f>
+        <v>406.75208460443361</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>322342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>889</v>
+      </c>
+      <c r="B37">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1776</v>
+      </c>
+      <c r="B38">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2672</v>
+      </c>
+      <c r="B39">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <f>1/B41</f>
+        <v>0.99800399201596801</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2">
+        <f>B32*B42</f>
+        <v>405.94020419604152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="2">
+        <v>322342</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>